<commit_message>
119 Random Event Data
</commit_message>
<xml_diff>
--- a/GameMaster/RPGTale/Data/Data_Excel/ExploreMetaData.xlsx
+++ b/GameMaster/RPGTale/Data/Data_Excel/ExploreMetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\建造工程\Project\GameMaster\RPGTale\Data\Data_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57672433-7147-40DF-98EA-BB991FBE393A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8C8194-B41D-45B7-9C74-A469713B8EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2055" windowWidth="26295" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="2295" windowWidth="24795" windowHeight="12510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExploreArea" sheetId="2" r:id="rId1"/>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD7B1E4-F0D7-4BD2-94C9-D21747820F10}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -921,7 +921,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BF95E4-A844-485D-B9D9-9F3997218EED}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1484,7 +1484,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
122 Explore Main Page
</commit_message>
<xml_diff>
--- a/GameMaster/RPGTale/Data/Data_Excel/ExploreMetaData.xlsx
+++ b/GameMaster/RPGTale/Data/Data_Excel/ExploreMetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\建造工程\Project\GameMaster\RPGTale\Data\Data_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87E3931-DA28-486D-A22D-476E9876DA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6845ED93-3B62-413F-952D-34F5C8FA52B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="810" windowWidth="24780" windowHeight="12510" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="2115" windowWidth="24780" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExploreArea" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>ExploreID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>SpriteOutput/RandomEvent/BG/RandomEvent_Pic_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unlock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExploreArea_Name_101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExploreArea_Desc_101</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD7B1E4-F0D7-4BD2-94C9-D21747820F10}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -704,10 +716,11 @@
     <col min="1" max="1" width="10.25" customWidth="1"/>
     <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="3" max="3" width="26.25" customWidth="1"/>
-    <col min="4" max="4" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -718,10 +731,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>100</v>
       </c>
@@ -731,24 +747,43 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>101</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="18" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -769,7 +804,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -946,7 +981,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D15" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1452,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1542,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{704E471A-C2F8-4396-A62B-F036FB8D977F}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>